<commit_message>
updated exp 3 codebook
</commit_message>
<xml_diff>
--- a/experiment 3/data/processed/codebook_processed_data.xlsx
+++ b/experiment 3/data/processed/codebook_processed_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiecummins/git/amp-intentionality/experiment 3/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE195DC8-EBBE-624D-B48B-8A7096A721E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F64DDDE-26BC-2F4D-83F1-8BE6F85AC2E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="2540" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8140" yWindow="2540" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="processed_data" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>variable</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>political affliliation of participants</t>
+  </si>
+  <si>
+    <t>valence type of prime: either Obama (B) or Trump (A).</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2500,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EE6269-E5B6-B846-B658-D01632BA4AF8}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2538,8 +2541,8 @@
       <c r="A4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>27</v>
+      <c r="B4" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
     </row>

</xml_diff>

<commit_message>
updated codebooks for exps 3 and 4
</commit_message>
<xml_diff>
--- a/experiment 3/data/processed/codebook_processed_data.xlsx
+++ b/experiment 3/data/processed/codebook_processed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiecummins/git/amp-intentionality/experiment 3/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F64DDDE-26BC-2F4D-83F1-8BE6F85AC2E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173E6CC5-231B-DB4A-A2C0-93ABFCBACD20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8140" yWindow="2540" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
     <t>political affliliation of participants</t>
   </si>
   <si>
-    <t>valence type of prime: either Obama (B) or Trump (A).</t>
+    <t>identity of the prime stimulus: either Obama (B) or Trump (A).</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2504,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>